<commit_message>
restore FP category, add some SPLASCH data as FP
</commit_message>
<xml_diff>
--- a/2022-05 HL7 May Connectathon/ConnectathonSampleData/Spreadsheets/Time Based Observations- Func Perf & SPLASCH.xlsx
+++ b/2022-05 HL7 May Connectathon/ConnectathonSampleData/Spreadsheets/Time Based Observations- Func Perf & SPLASCH.xlsx
@@ -3158,7 +3158,7 @@
     <t>HHA-PF-SOC-OASIS-2A-Ob-Question-4</t>
   </si>
   <si>
-    <t xml:space="preserve">mental-functions </t>
+    <t xml:space="preserve">mental-functions</t>
   </si>
   <si>
     <t>HHA-SC-DG-OASIS-2C</t>
@@ -3470,7 +3470,7 @@
     <t>BSJ-ObservationSPLASCH-133</t>
   </si>
   <si>
-    <t>BSJ-patientBSJ1</t>
+    <t>patientBSJ1</t>
   </si>
   <si>
     <t>digestive-metabolic-endocrine-systems</t>

</xml_diff>